<commit_message>
Attempt to fix issue with xls file.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_12_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_12_0.xlsx
@@ -9564,9 +9564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1560960</xdr:colOff>
+      <xdr:colOff>1560600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9581,7 +9581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="28440"/>
-          <a:ext cx="1484640" cy="543960"/>
+          <a:ext cx="1484280" cy="543600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9598,7 +9598,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Taxons" displayName="Taxons" ref="G2:G19" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="G2:G19"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Column1"/>
   </tableColumns>

</xml_diff>

<commit_message>
Leave cursor at A1 cell
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v3_12_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v3_12_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckostiw/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A96EB6-7FD9-1146-A6D2-C19F6018D96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E54B62-D363-A04B-A891-B38D51D44727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30200" yWindow="-3100" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10062,9 +10062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE500"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>